<commit_message>
Values updated Excel Sheet
Values updated Excel Sheet
</commit_message>
<xml_diff>
--- a/Submission/PerformanceReport_Push-Sum_Gossip.xlsx
+++ b/Submission/PerformanceReport_Push-Sum_Gossip.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="gossip" sheetId="1" r:id="rId1"/>
@@ -230,10 +230,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -639,11 +639,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2143698912"/>
-        <c:axId val="2143699456"/>
+        <c:axId val="-1592157760"/>
+        <c:axId val="-1593908576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2143698912"/>
+        <c:axId val="-1592157760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -742,7 +742,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143699456"/>
+        <c:crossAx val="-1593908576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -750,7 +750,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143699456"/>
+        <c:axId val="-1593908576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,7 +874,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143698912"/>
+        <c:crossAx val="-1592157760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1000"/>
@@ -1181,11 +1181,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="195736336"/>
-        <c:axId val="195744496"/>
+        <c:axId val="-1417645840"/>
+        <c:axId val="-1417644208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195736336"/>
+        <c:axId val="-1417645840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1287,7 +1287,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195744496"/>
+        <c:crossAx val="-1417644208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1295,7 +1295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195744496"/>
+        <c:axId val="-1417644208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1419,7 +1419,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195736336"/>
+        <c:crossAx val="-1417645840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1000"/>
@@ -1757,11 +1757,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2143701088"/>
-        <c:axId val="2143701632"/>
+        <c:axId val="-1418252848"/>
+        <c:axId val="-1418250672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2143701088"/>
+        <c:axId val="-1418252848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1860,7 +1860,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143701632"/>
+        <c:crossAx val="-1418250672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1868,7 +1868,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143701632"/>
+        <c:axId val="-1418250672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1992,7 +1992,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143701088"/>
+        <c:crossAx val="-1418252848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1000"/>
@@ -2330,11 +2330,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="195156496"/>
-        <c:axId val="195164656"/>
+        <c:axId val="-1418244144"/>
+        <c:axId val="-1418259376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195156496"/>
+        <c:axId val="-1418244144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2433,7 +2433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195164656"/>
+        <c:crossAx val="-1418259376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2441,7 +2441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195164656"/>
+        <c:axId val="-1418259376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2565,7 +2565,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195156496"/>
+        <c:crossAx val="-1418244144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1000"/>
@@ -2903,11 +2903,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="195154864"/>
-        <c:axId val="195155408"/>
+        <c:axId val="-1418245776"/>
+        <c:axId val="-1418256112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195154864"/>
+        <c:axId val="-1418245776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3006,7 +3006,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195155408"/>
+        <c:crossAx val="-1418256112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3014,7 +3014,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195155408"/>
+        <c:axId val="-1418256112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3138,7 +3138,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195154864"/>
+        <c:crossAx val="-1418245776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1000"/>
@@ -3476,11 +3476,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="195163024"/>
-        <c:axId val="195161392"/>
+        <c:axId val="-1418249584"/>
+        <c:axId val="-1418245232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195163024"/>
+        <c:axId val="-1418249584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3579,7 +3579,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195161392"/>
+        <c:crossAx val="-1418245232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3587,7 +3587,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195161392"/>
+        <c:axId val="-1418245232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3711,7 +3711,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195163024"/>
+        <c:crossAx val="-1418249584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1000"/>
@@ -4218,11 +4218,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="195165744"/>
-        <c:axId val="195157040"/>
+        <c:axId val="-1418253392"/>
+        <c:axId val="-1418247408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195165744"/>
+        <c:axId val="-1418253392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4315,7 +4315,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195157040"/>
+        <c:crossAx val="-1418247408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4323,7 +4323,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195157040"/>
+        <c:axId val="-1418247408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4510,7 +4510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195165744"/>
+        <c:crossAx val="-1418253392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1000"/>
@@ -4845,11 +4845,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="195155952"/>
-        <c:axId val="195158128"/>
+        <c:axId val="-1418257744"/>
+        <c:axId val="-1418249040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195155952"/>
+        <c:axId val="-1418257744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4951,7 +4951,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195158128"/>
+        <c:crossAx val="-1418249040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4959,7 +4959,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195158128"/>
+        <c:axId val="-1418249040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5083,7 +5083,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195155952"/>
+        <c:crossAx val="-1418257744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1000"/>
@@ -5429,11 +5429,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="195166832"/>
-        <c:axId val="195159216"/>
+        <c:axId val="-1417642576"/>
+        <c:axId val="-1417637680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195166832"/>
+        <c:axId val="-1417642576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5535,7 +5535,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195159216"/>
+        <c:crossAx val="-1417637680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5543,7 +5543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195159216"/>
+        <c:axId val="-1417637680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5658,7 +5658,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195166832"/>
+        <c:crossAx val="-1417642576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5998,11 +5998,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="195743408"/>
-        <c:axId val="195734704"/>
+        <c:axId val="-1417640944"/>
+        <c:axId val="-1417646384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195743408"/>
+        <c:axId val="-1417640944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6104,7 +6104,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195734704"/>
+        <c:crossAx val="-1417646384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6112,7 +6112,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195734704"/>
+        <c:axId val="-1417646384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6236,7 +6236,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195743408"/>
+        <c:crossAx val="-1417640944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12857,7 +12857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E19" sqref="E19:E21"/>
     </sheetView>
   </sheetViews>
@@ -12892,7 +12892,7 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="8">
@@ -12901,7 +12901,7 @@
       <c r="D2" s="7">
         <v>30212</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>9</v>
       </c>
     </row>
@@ -12909,27 +12909,27 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="8">
         <v>729</v>
       </c>
       <c r="D3" s="7">
         <v>35622</v>
       </c>
-      <c r="E3" s="18"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="8">
         <v>1000</v>
       </c>
       <c r="D4" s="7">
         <v>88499</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="19" t="s">
         <v>12</v>
       </c>
     </row>
@@ -12937,33 +12937,33 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="8">
         <v>2197</v>
       </c>
       <c r="D5" s="7">
         <v>200836</v>
       </c>
-      <c r="E5" s="18"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="8">
         <v>3375</v>
       </c>
       <c r="D6" s="7">
         <v>275356</v>
       </c>
-      <c r="E6" s="18"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="8">
@@ -12972,7 +12972,7 @@
       <c r="D7" s="7">
         <v>2634</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="19" t="s">
         <v>10</v>
       </c>
     </row>
@@ -12980,7 +12980,7 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="8">
@@ -12989,13 +12989,13 @@
       <c r="D8" s="7">
         <v>2815</v>
       </c>
-      <c r="E8" s="18"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="8">
@@ -13004,7 +13004,7 @@
       <c r="D9" s="7">
         <v>3782</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -13012,7 +13012,7 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="8">
@@ -13021,13 +13021,13 @@
       <c r="D10" s="7">
         <v>19610</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="8">
@@ -13036,13 +13036,13 @@
       <c r="D11" s="7">
         <v>62948</v>
       </c>
-      <c r="E11" s="18"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="8">
@@ -13051,7 +13051,7 @@
       <c r="D12" s="7">
         <v>2147</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="19" t="s">
         <v>13</v>
       </c>
     </row>
@@ -13059,7 +13059,7 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="8">
@@ -13068,13 +13068,13 @@
       <c r="D13" s="7">
         <v>2534</v>
       </c>
-      <c r="E13" s="18"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="8">
@@ -13083,7 +13083,7 @@
       <c r="D14" s="7">
         <v>2616</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="19" t="s">
         <v>14</v>
       </c>
     </row>
@@ -13091,7 +13091,7 @@
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="8">
@@ -13100,13 +13100,13 @@
       <c r="D15" s="7">
         <v>3141</v>
       </c>
-      <c r="E15" s="18"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="8">
@@ -13115,13 +13115,13 @@
       <c r="D16" s="7">
         <v>3511</v>
       </c>
-      <c r="E16" s="18"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="8">
@@ -13130,7 +13130,7 @@
       <c r="D17" s="7">
         <v>2128</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="19" t="s">
         <v>13</v>
       </c>
     </row>
@@ -13138,7 +13138,7 @@
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="8">
@@ -13147,13 +13147,13 @@
       <c r="D18" s="7">
         <v>2519</v>
       </c>
-      <c r="E18" s="18"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="8">
@@ -13162,7 +13162,7 @@
       <c r="D19" s="7">
         <v>2603</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="19" t="s">
         <v>26</v>
       </c>
     </row>
@@ -13170,7 +13170,7 @@
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="8">
@@ -13179,13 +13179,13 @@
       <c r="D20" s="7">
         <v>2957</v>
       </c>
-      <c r="E20" s="18"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="8">
@@ -13194,7 +13194,7 @@
       <c r="D21" s="7">
         <v>2897</v>
       </c>
-      <c r="E21" s="18"/>
+      <c r="E21" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -13256,7 +13256,7 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="8">
@@ -13265,7 +13265,7 @@
       <c r="D2" s="7">
         <v>8540</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>9</v>
       </c>
     </row>
@@ -13273,27 +13273,27 @@
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="8">
         <v>729</v>
       </c>
       <c r="D3" s="7">
         <v>16701</v>
       </c>
-      <c r="E3" s="18"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="8">
         <v>1000</v>
       </c>
       <c r="D4" s="7">
         <v>21521</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="19" t="s">
         <v>15</v>
       </c>
     </row>
@@ -13301,33 +13301,33 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="8">
         <v>2197</v>
       </c>
       <c r="D5" s="7">
         <v>32025</v>
       </c>
-      <c r="E5" s="18"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="8">
         <v>3375</v>
       </c>
       <c r="D6" s="7">
         <v>54907</v>
       </c>
-      <c r="E6" s="18"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="8">
@@ -13336,7 +13336,7 @@
       <c r="D7" s="7">
         <v>170</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="19" t="s">
         <v>16</v>
       </c>
     </row>
@@ -13344,7 +13344,7 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="8">
@@ -13353,13 +13353,13 @@
       <c r="D8" s="7">
         <v>176</v>
       </c>
-      <c r="E8" s="18"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="8">
@@ -13368,7 +13368,7 @@
       <c r="D9" s="7">
         <v>191</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="19" t="s">
         <v>17</v>
       </c>
     </row>
@@ -13376,7 +13376,7 @@
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="8">
@@ -13385,13 +13385,13 @@
       <c r="D10" s="7">
         <v>288</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="8">
@@ -13400,13 +13400,13 @@
       <c r="D11" s="7">
         <v>406</v>
       </c>
-      <c r="E11" s="18"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="8">
@@ -13415,7 +13415,7 @@
       <c r="D12" s="7">
         <v>587</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="19" t="s">
         <v>10</v>
       </c>
     </row>
@@ -13423,7 +13423,7 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="8">
@@ -13432,13 +13432,13 @@
       <c r="D13" s="7">
         <v>882</v>
       </c>
-      <c r="E13" s="18"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="8">
@@ -13447,7 +13447,7 @@
       <c r="D14" s="7">
         <v>1300</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="19" t="s">
         <v>18</v>
       </c>
     </row>
@@ -13455,7 +13455,7 @@
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="8">
@@ -13464,13 +13464,13 @@
       <c r="D15" s="7">
         <v>4542</v>
       </c>
-      <c r="E15" s="18"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="8">
@@ -13479,13 +13479,13 @@
       <c r="D16" s="7">
         <v>10209</v>
       </c>
-      <c r="E16" s="18"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="8">
@@ -13494,7 +13494,7 @@
       <c r="D17" s="7">
         <v>141</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="19" t="s">
         <v>19</v>
       </c>
     </row>
@@ -13502,7 +13502,7 @@
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="8">
@@ -13511,13 +13511,13 @@
       <c r="D18" s="7">
         <v>195</v>
       </c>
-      <c r="E18" s="18"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="8">
@@ -13526,7 +13526,7 @@
       <c r="D19" s="7">
         <v>273</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="19" t="s">
         <v>20</v>
       </c>
     </row>
@@ -13534,7 +13534,7 @@
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="8">
@@ -13543,13 +13543,13 @@
       <c r="D20" s="7">
         <v>622</v>
       </c>
-      <c r="E20" s="18"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="8">
@@ -13558,7 +13558,7 @@
       <c r="D21" s="7">
         <v>799</v>
       </c>
-      <c r="E21" s="18"/>
+      <c r="E21" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -13585,8 +13585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -13652,8 +13652,12 @@
       <c r="A6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
+      <c r="B6" s="16">
+        <v>500000</v>
+      </c>
+      <c r="C6" s="17">
+        <v>138</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="21"/>

</xml_diff>